<commit_message>
update table and figures
</commit_message>
<xml_diff>
--- a/HJA_sjSDM_paper/paper/Table S_Predictors.xlsx
+++ b/HJA_sjSDM_paper/paper/Table S_Predictors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UEA\gitHRepos\HJA_analyses_Kelpie\HJA_sjSDM_paper\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3158B3-FB9C-438E-BC74-28410D035BD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF02A448-DCD0-479C-AA7D-78FF9DB97BCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29913" yWindow="1152" windowWidth="18851" windowHeight="9844" xr2:uid="{1F5AF100-70DA-4190-8C9E-773A29E62371}"/>
+    <workbookView xWindow="25017" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{1F5AF100-70DA-4190-8C9E-773A29E62371}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="169">
   <si>
     <t>be30</t>
   </si>
@@ -539,6 +539,12 @@
   </si>
   <si>
     <t>HJA</t>
+  </si>
+  <si>
+    <t>Canopy height (25th percentile)</t>
+  </si>
+  <si>
+    <t>Canopy height (95th percentile)</t>
   </si>
 </sst>
 </file>
@@ -901,13 +907,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17AF1E92-1A70-4317-8820-8C19077DC4C1}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
     <col min="2" max="2" width="37.21875" customWidth="1"/>
     <col min="3" max="3" width="73.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
@@ -949,7 +955,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -963,7 +969,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -1831,6 +1837,7 @@
     <sortCondition ref="A2:A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update predictor table S_predictors
</commit_message>
<xml_diff>
--- a/HJA_sjSDM_paper/paper/Table S_Predictors.xlsx
+++ b/HJA_sjSDM_paper/paper/Table S_Predictors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UEA\gitHRepos\HJA_analyses_Kelpie\HJA_sjSDM_paper\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC54D191-30AE-4349-9BD7-539B1B0BDB9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D861CEBB-E1A7-4C69-8F6C-B6D94C3C1FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25017" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{1F5AF100-70DA-4190-8C9E-773A29E62371}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1F5AF100-70DA-4190-8C9E-773A29E62371}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="193">
   <si>
     <t>be30</t>
   </si>
@@ -593,6 +593,30 @@
   </si>
   <si>
     <t>5% percentile of annual NDVI averaged over 500m radius</t>
+  </si>
+  <si>
+    <t>TPI (Topographic Position Index) is the difference between the value of a central cell and the mean value of its surrounding cells within 1 km window. - raster package</t>
+  </si>
+  <si>
+    <t>TPI (Topographic Position Index) is the difference between the value of the central cell and the mean value of its surrounding cells within 250m window. - raster package</t>
+  </si>
+  <si>
+    <t>TPI (Topographic Position Index) is the difference between the value of the central cell and the mean value of its surrounding cells within 500 m window - raster package</t>
+  </si>
+  <si>
+    <t>topographic wetness index represents a theoretical estimation of the accumulation of flow at any point (ie depends on upstream catchment area). Formula: ln(a/tan(beta)); (a = upslope contributing area per unit contour; tan(beta) = local slope angle)</t>
+  </si>
+  <si>
+    <t>NBR: Normalised Burn Ratio - identify burn areas and severity of burn</t>
+  </si>
+  <si>
+    <t>NDMI: Normalised Difference Moisture Index, for vegetation water content</t>
+  </si>
+  <si>
+    <t>From Oregon shapefile of logged areas over last ~ 100 years</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -953,13 +977,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17AF1E92-1A70-4317-8820-8C19077DC4C1}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E59" sqref="A1:E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.5546875" customWidth="1"/>
     <col min="2" max="2" width="37.21875" customWidth="1"/>
@@ -967,7 +991,7 @@
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -983,8 +1007,11 @@
       <c r="E1" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -998,7 +1025,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1012,7 +1039,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1026,7 +1053,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1043,7 +1070,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1060,7 +1087,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1077,7 +1104,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1094,7 +1121,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1108,7 +1135,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1125,7 +1152,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1139,7 +1166,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1156,7 +1183,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1173,7 +1200,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1190,7 +1217,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1204,7 +1231,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1220,8 +1247,11 @@
       <c r="E16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1237,8 +1267,11 @@
       <c r="E17" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1251,8 +1284,11 @@
       <c r="D18" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1269,7 +1305,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1285,8 +1321,11 @@
       <c r="E20" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -1303,7 +1342,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -1317,7 +1356,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -1331,7 +1370,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1345,7 +1384,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -1362,7 +1401,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1376,7 +1415,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1392,8 +1431,11 @@
       <c r="E27" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -1407,7 +1449,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -1421,7 +1463,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -1435,7 +1477,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -1449,7 +1491,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -1463,7 +1505,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -1477,7 +1519,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -1491,7 +1533,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -1505,7 +1547,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -1522,7 +1564,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -1536,7 +1578,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -1550,7 +1592,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1563,8 +1605,11 @@
       <c r="D39" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1578,7 +1623,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -1592,7 +1637,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -1609,7 +1654,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -1623,7 +1668,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -1640,7 +1685,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -1657,7 +1702,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -1671,7 +1716,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>68</v>
       </c>
@@ -1688,7 +1733,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -1702,7 +1747,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -1716,7 +1761,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -1730,7 +1775,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -1747,7 +1792,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -1764,7 +1809,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -1778,7 +1823,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -1794,8 +1839,11 @@
       <c r="E54" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -1812,7 +1860,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -1826,7 +1874,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -1843,7 +1891,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1860,7 +1908,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>124</v>
       </c>
@@ -1897,7 +1945,7 @@
       <selection sqref="A1:A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>